<commit_message>
radix with work efficient scan and added flag to trigger class example or run on full test array
</commit_message>
<xml_diff>
--- a/Project2-Character-Recognition/2x2_XOR_excel_example.xlsx
+++ b/Project2-Character-Recognition/2x2_XOR_excel_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanbo\OneDrive\Desktop\Project2-Stream-Compaction-master\Project2-Character-Recognition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klayPC\Documents\github\gpu-programming\Project2-Number-Algorithms\Project2-Character-Recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B98C44B4-B8A5-4E7D-896A-1EB4BAB1F08B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A977544B-AE65-4D63-B966-8BC4BD3109B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27120" yWindow="5400" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1219,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>